<commit_message>
fix convert nested xlsx back to the same input json
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -375,90 +375,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A0:F14"/>
+  <dimension ref="A0:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>name</v>
+        <v>data</v>
       </c>
       <c r="B1" t="str">
-        <v>breed</v>
+        <v>data.name</v>
       </c>
       <c r="C1" t="str">
-        <v>age</v>
+        <v>data.breed</v>
       </c>
       <c r="D1" t="str">
-        <v>origin</v>
+        <v>data.age</v>
       </c>
       <c r="E1" t="str">
-        <v>origin.country</v>
+        <v>data.origin</v>
       </c>
       <c r="F1" t="str">
-        <v>origin.city</v>
+        <v>data.origin.country</v>
+      </c>
+      <c r="G1" t="str">
+        <v>data.origin.city</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
+      <c r="B2" t="str">
         <v>dog1</v>
       </c>
-      <c r="B2" t="str">
+      <c r="C2" t="str">
         <v>dog</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>2</v>
       </c>
-      <c r="E2" t="str">
+      <c r="F2" t="str">
         <v>TH</v>
       </c>
-      <c r="F2" t="str">
+      <c r="G2" t="str">
         <v>BKK</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="str">
+      <c r="B3" t="str">
         <v>bird1</v>
       </c>
-      <c r="B3" t="str">
+      <c r="C3" t="str">
         <v>bird</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" t="str">
+      <c r="F3" t="str">
         <v>TH</v>
       </c>
-      <c r="F3" t="str">
+      <c r="G3" t="str">
         <v>BKK</v>
       </c>
     </row>
     <row r="4">
-      <c r="E4" t="str">
-        <v>US</v>
+      <c r="B4" t="str">
+        <v>cat1</v>
+      </c>
+      <c r="C4" t="str">
+        <v>cat</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="F4" t="str">
+        <v>TH</v>
+      </c>
+      <c r="G4" t="str">
+        <v>CNX</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="str">
-        <v>cat1</v>
-      </c>
       <c r="B5" t="str">
-        <v>cat</v>
-      </c>
-      <c r="C5">
-        <v>7</v>
-      </c>
-      <c r="E5" t="str">
+        <v>bird1</v>
+      </c>
+      <c r="C5" t="str">
+        <v>bird</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="str">
         <v>TH</v>
-      </c>
-      <c r="F5" t="str">
-        <v>CNX</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A0:F14"/>
+    <ignoredError numberStoredAsText="1" sqref="A0:G6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix nested array error
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -375,60 +375,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A0:G6"/>
+  <dimension ref="A0:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>data</v>
+        <v>myData_isArray</v>
       </c>
       <c r="B1" t="str">
-        <v>data.name</v>
+        <v>myData_isArray.name</v>
       </c>
       <c r="C1" t="str">
-        <v>data.breed</v>
+        <v>myData_isArray.breed</v>
       </c>
       <c r="D1" t="str">
-        <v>data.age</v>
+        <v>myData_isArray.age</v>
       </c>
       <c r="E1" t="str">
-        <v>data.origin</v>
+        <v>myData_isArray.origin</v>
       </c>
       <c r="F1" t="str">
-        <v>data.origin.country</v>
+        <v>myData_isArray.origin.country</v>
       </c>
       <c r="G1" t="str">
-        <v>data.origin.city</v>
+        <v>myData_isArray.origin.city</v>
+      </c>
+      <c r="H1" t="str">
+        <v>myData_isArray.test</v>
+      </c>
+      <c r="I1" t="str">
+        <v>myData_isArray.array_ja_isArray</v>
+      </c>
+      <c r="J1" t="str">
+        <v>myData_isArray.array_ja_isArray.test</v>
+      </c>
+      <c r="K1" t="str">
+        <v>myData_isArray.array_ja_isArray.test2</v>
+      </c>
+      <c r="L1" t="str">
+        <v>myData_isArray.test_age</v>
       </c>
     </row>
     <row r="2">
-      <c r="B2" t="str">
-        <v>dog1</v>
-      </c>
-      <c r="C2" t="str">
-        <v>dog</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="F2" t="str">
-        <v>TH</v>
-      </c>
-      <c r="G2" t="str">
-        <v>BKK</v>
+      <c r="A2" t="str">
+        <v>[4]</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="str">
-        <v>bird1</v>
+        <v>dog1</v>
       </c>
       <c r="C3" t="str">
-        <v>bird</v>
+        <v>dog</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="str">
         <v>TH</v>
@@ -439,38 +442,77 @@
     </row>
     <row r="4">
       <c r="B4" t="str">
-        <v>cat1</v>
+        <v>bird1</v>
       </c>
       <c r="C4" t="str">
-        <v>cat</v>
+        <v>bird</v>
       </c>
       <c r="D4">
-        <v>7</v>
-      </c>
-      <c r="F4" t="str">
-        <v>TH</v>
+        <v>1</v>
       </c>
       <c r="G4" t="str">
-        <v>CNX</v>
+        <v>BKK</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="str">
-        <v>bird1</v>
+        <v>cat1</v>
       </c>
       <c r="C5" t="str">
-        <v>bird</v>
+        <v>cat</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F5" t="str">
         <v>TH</v>
       </c>
+      <c r="G5" t="str">
+        <v>BKK</v>
+      </c>
+      <c r="H5" t="str">
+        <v>ok</v>
+      </c>
+      <c r="I5" t="str">
+        <v>[2]</v>
+      </c>
+      <c r="L5">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6" t="str">
+        <v>qwerty</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7" t="str">
+        <v>qwerty2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="str">
+        <v>bird2</v>
+      </c>
+      <c r="C8" t="str">
+        <v>bird</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="str">
+        <v>TH</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A0:G6"/>
+    <ignoredError numberStoredAsText="1" sqref="A0:L9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>